<commit_message>
Add deduplication notebook and sample data files
</commit_message>
<xml_diff>
--- a/notebooks/output/deduped_contacts.xlsx
+++ b/notebooks/output/deduped_contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd893d932ac0802d/Projects/data-dedup-pilot/notebooks/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_4A482F572B77854633A6F7A6AB5484D3D212F28D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D5BF468-0898-4387-9ED2-75C713556FA2}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_4A482F572B570E1ADB87E1A6AB5484D3D212F28D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD6FFF27-1B9E-4850-AD21-D310406531CC}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="870" windowWidth="23805" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1230,14 +1230,12 @@
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>